<commit_message>
add Attendancelimit column in execl while import data
</commit_message>
<xml_diff>
--- a/HRMS.UI/wwwroot/SampleTemplates/EmployeeMasterUpdate.xlsx
+++ b/HRMS.UI/wwwroot/SampleTemplates/EmployeeMasterUpdate.xlsx
@@ -24,18 +24,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Alpha_Emp_Code</t>
   </si>
   <si>
-    <t xml:space="preserve">    Designation_Name</t>
+    <t>Account Executive</t>
   </si>
   <si>
-    <t xml:space="preserve">  Reporting_Manager_Code</t>
+    <t>Designation_Name</t>
   </si>
   <si>
-    <t>Account Executive</t>
+    <t>Reporting_Manager_Code</t>
+  </si>
+  <si>
+    <t>AttendanceLimit</t>
   </si>
 </sst>
 </file>
@@ -353,10 +356,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -364,28 +367,35 @@
     <col min="1" max="1" width="21.26953125" customWidth="1"/>
     <col min="2" max="2" width="23.6328125" customWidth="1"/>
     <col min="3" max="3" width="26" customWidth="1"/>
+    <col min="4" max="4" width="17.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>10782</v>
+      </c>
+      <c r="B2" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>10675</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
       </c>
       <c r="C2">
         <v>10781</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>